<commit_message>
Add check chord type function to check if chord type is minor or diminished
</commit_message>
<xml_diff>
--- a/music21_project/last.xlsx
+++ b/music21_project/last.xlsx
@@ -1362,7 +1362,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3774,7 +3774,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>17</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
@@ -4042,7 +4042,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -4310,7 +4310,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>19</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -4511,7 +4511,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>19</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -6052,7 +6052,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -6186,7 +6186,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -6253,7 +6253,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">

</xml_diff>